<commit_message>
hypothesis testing example added
</commit_message>
<xml_diff>
--- a/python/eda/Post-read/data_quality_report.xlsx
+++ b/python/eda/Post-read/data_quality_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/Work/Vired/Content/self_paced/code_repo/python/eda/Post-read/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{DDE1EDFA-0032-1940-B500-2F64ED8FB9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5772A27B-7BE3-6E40-833E-6C0E38A85414}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{DDE1EDFA-0032-1940-B500-2F64ED8FB9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9F57D77-429F-E147-9C6D-9576AB7193AE}"/>
   <bookViews>
     <workbookView xWindow="260" yWindow="500" windowWidth="28040" windowHeight="15520" xr2:uid="{C1E21C51-26D5-964F-A9E4-E7BD232BE2C2}"/>
   </bookViews>
@@ -102,11 +102,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>1. Two distinct values
-2. Makes are more than females
-3. 23% missing values</t>
-  </si>
-  <si>
     <t>birthyear</t>
   </si>
   <si>
@@ -114,6 +109,11 @@
 2. No zero values
 3. Missing values are 23%
 4. 5th percentile is 1959, makes sense given the current demographics</t>
+  </si>
+  <si>
+    <t>1. Two distinct values
+2. Males are more than females
+3. 23% missing values</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAF3534-31DB-C14B-925D-9D5B1D85CBBE}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="209" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="209" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,15 +598,15 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>